<commit_message>
main program og 2 hjalparprogram virka
</commit_message>
<xml_diff>
--- a/reports/OSByggingar.xlsx
+++ b/reports/OSByggingar.xlsx
@@ -51,10 +51,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,58 +433,52 @@
     <col width="13" bestFit="1" customWidth="1" min="3" max="3"/>
     <col width="13" bestFit="1" customWidth="1" min="4" max="4"/>
     <col width="13" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="13" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="13" bestFit="1" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Date: 2025-06-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
           <t>Employee</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
         <is>
           <t>Clock In</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F2" s="2" t="inlineStr">
         <is>
           <t>Clock Out</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G2" s="2" t="inlineStr">
         <is>
           <t>Hours Worked</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>olafur</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2025-06-16</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>11:12:00</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>11:13:00</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>0.02</v>
       </c>
     </row>
     <row r="3">
@@ -495,39 +489,166 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-16</t>
+          <t>Oli saer</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>20:16:00</t>
+          <t>Akureyri</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>20:19:00</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>0.05</v>
+          <t>Foundation prep</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>09:16</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>09:27</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>0.18</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>olafur</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Oli saer</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Reykjavik</t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Total Hours:</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
+          <t>Pour concrete</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>09:45</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>09:49</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="5">
-      <c r="D5" s="2" t="n"/>
-      <c r="E5" s="2" t="n"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>olafur</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Oli saer</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Akureyri</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Foundation prep</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>12:03</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>12:03</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" s="1" t="inlineStr">
+        <is>
+          <t>Total: 0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Overall Total Hours: 0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="G9" s="1" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>Task Name</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>Total Hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Foundation prep</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Pour concrete</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.07000000000000001</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>